<commit_message>
Created new document with summary of models
</commit_message>
<xml_diff>
--- a/Fecal_StableIsotope_estimates.xlsx
+++ b/Fecal_StableIsotope_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amikk\Documents\Rprojects\Diet-sensitivty-to-TDFs-and-priors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B57543-FB38-440F-961C-1A85C272C23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FDF332-AE11-4719-9FF1-B18134E95933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46335" yWindow="135" windowWidth="28800" windowHeight="15300" xr2:uid="{0AF0228D-C091-4D99-845D-2DD8AA361D61}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0AF0228D-C091-4D99-845D-2DD8AA361D61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,13 +439,13 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -448,7 +453,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -459,7 +464,7 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>0.18</v>
       </c>
       <c r="C2" t="s">
@@ -468,64 +473,64 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.314</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.22</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1">
-        <v>6.5000000000000002E-2</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4.6000000000000006E-2</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.01</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.19833333333333333</v>
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.4</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.22</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.314</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>0.2535</v>
       </c>
       <c r="C8" t="s">
@@ -534,64 +539,64 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.47299999999999998</v>
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8.6500000000000007E-2</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.23699999999999999</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.13650000000000001</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <v>9.849999999999999E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.2</v>
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1">
-        <v>8.6500000000000007E-2</v>
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.47299999999999998</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>0.13500000000000001</v>
       </c>
       <c r="C14" t="s">
@@ -600,64 +605,64 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0.16666666666666669</v>
+        <v>11</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.28799999999999998</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.09</v>
+        <v>12</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.01</v>
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4.6000000000000006E-2</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.23699999999999999</v>
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.28799999999999998</v>
+        <v>10</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.16666666666666669</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>3.3333333333333332E-4</v>
       </c>
       <c r="C20" t="s">
@@ -666,64 +671,64 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="1">
-        <v>3.3333333333333333E-2</v>
+        <v>12</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.39600000000000002</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.4</v>
+        <v>9</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.19833333333333333</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="1">
-        <v>9.849999999999999E-2</v>
+        <v>3</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.13650000000000001</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>10</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.09</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0.39600000000000002</v>
+        <v>11</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>0.45633333333333331</v>
       </c>
       <c r="C26" t="s">
@@ -732,7 +737,6 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C26">
-    <sortCondition ref="A2:A26"/>
     <sortCondition ref="C2:C26"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>